<commit_message>
Implemented junit for addTest.
</commit_message>
<xml_diff>
--- a/Testcases/Calculator_Testcase.xlsx
+++ b/Testcases/Calculator_Testcase.xlsx
@@ -15,6 +15,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$I$98</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="118">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -270,9 +273,6 @@
     <t>average value should be displayed</t>
   </si>
   <si>
-    <t>2,4,6,8,10</t>
-  </si>
-  <si>
     <t>Give five  integer value in array</t>
   </si>
   <si>
@@ -282,9 +282,6 @@
     <t>Give four integer value and one float value in array</t>
   </si>
   <si>
-    <t>1,3,5,7,1.2</t>
-  </si>
-  <si>
     <t>3.44'</t>
   </si>
   <si>
@@ -294,12 +291,6 @@
     <t>Give four integer value and one fraction value in array</t>
   </si>
   <si>
-    <t>1,3,5,7,1/2</t>
-  </si>
-  <si>
-    <t>3.5'</t>
-  </si>
-  <si>
     <t>TC_15</t>
   </si>
   <si>
@@ -358,6 +349,39 @@
   </si>
   <si>
     <t>multiplication should not be perform</t>
+  </si>
+  <si>
+    <t>"1,3,5,7,1.2"</t>
+  </si>
+  <si>
+    <t>"2,4,6,8,10"</t>
+  </si>
+  <si>
+    <t>"1,3,5,7,1/2"</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>3.3'</t>
+  </si>
+  <si>
+    <t>Not yet implemented</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Not Run</t>
+  </si>
+  <si>
+    <t>Infinity displayed instead of error</t>
   </si>
 </sst>
 </file>
@@ -691,15 +715,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G98"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K68" sqref="K68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -721,8 +745,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -733,7 +763,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D3" t="s">
         <v>10</v>
       </c>
@@ -743,8 +773,11 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>13</v>
       </c>
@@ -754,8 +787,11 @@
       <c r="G4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>16</v>
       </c>
@@ -765,8 +801,11 @@
       <c r="G5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>18</v>
       </c>
@@ -776,8 +815,11 @@
       <c r="G6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -788,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>23</v>
       </c>
@@ -798,8 +840,11 @@
       <c r="G8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>25</v>
       </c>
@@ -809,8 +854,11 @@
       <c r="G9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>16</v>
       </c>
@@ -820,8 +868,11 @@
       <c r="G10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>18</v>
       </c>
@@ -831,8 +882,11 @@
       <c r="G11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -843,7 +897,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>10</v>
       </c>
@@ -853,8 +907,11 @@
       <c r="G13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>13</v>
       </c>
@@ -864,8 +921,11 @@
       <c r="G14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>29</v>
       </c>
@@ -875,8 +935,11 @@
       <c r="G15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>18</v>
       </c>
@@ -886,8 +949,11 @@
       <c r="G16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -898,7 +964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>23</v>
       </c>
@@ -908,8 +974,11 @@
       <c r="G18" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>25</v>
       </c>
@@ -919,8 +988,11 @@
       <c r="G19" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D20" t="s">
         <v>29</v>
       </c>
@@ -930,8 +1002,11 @@
       <c r="G20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D21" t="s">
         <v>18</v>
       </c>
@@ -941,8 +1016,11 @@
       <c r="G21" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -953,7 +1031,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D23" t="s">
         <v>42</v>
       </c>
@@ -963,8 +1041,11 @@
       <c r="G23" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D24" t="s">
         <v>43</v>
       </c>
@@ -974,8 +1055,11 @@
       <c r="G24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D25" t="s">
         <v>29</v>
       </c>
@@ -985,8 +1069,11 @@
       <c r="G25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D26" t="s">
         <v>18</v>
       </c>
@@ -996,8 +1083,11 @@
       <c r="G26" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1005,7 +1095,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>44</v>
       </c>
@@ -1015,8 +1105,11 @@
       <c r="G28" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>45</v>
       </c>
@@ -1026,16 +1119,22 @@
       <c r="G29">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
         <v>29</v>
       </c>
       <c r="E30" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>18</v>
       </c>
@@ -1045,8 +1144,11 @@
       <c r="G31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1057,7 +1159,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>10</v>
       </c>
@@ -1067,8 +1169,11 @@
       <c r="G33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>13</v>
       </c>
@@ -1078,8 +1183,11 @@
       <c r="G34" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>49</v>
       </c>
@@ -1089,8 +1197,11 @@
       <c r="G35" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>18</v>
       </c>
@@ -1100,8 +1211,11 @@
       <c r="G36">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1112,7 +1226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>23</v>
       </c>
@@ -1122,8 +1236,11 @@
       <c r="G38" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>25</v>
       </c>
@@ -1133,8 +1250,11 @@
       <c r="G39" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>49</v>
       </c>
@@ -1144,8 +1264,11 @@
       <c r="G40" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>18</v>
       </c>
@@ -1155,8 +1278,11 @@
       <c r="G41" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -1164,7 +1290,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
         <v>44</v>
       </c>
@@ -1174,8 +1300,11 @@
       <c r="G43" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D44" t="s">
         <v>45</v>
       </c>
@@ -1185,16 +1314,22 @@
       <c r="G44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>49</v>
       </c>
       <c r="E45" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>18</v>
       </c>
@@ -1204,8 +1339,11 @@
       <c r="G46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>71</v>
       </c>
@@ -1216,7 +1354,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D48" t="s">
         <v>10</v>
       </c>
@@ -1226,8 +1364,11 @@
       <c r="G48" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D49" t="s">
         <v>13</v>
       </c>
@@ -1237,8 +1378,11 @@
       <c r="G49" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D50" t="s">
         <v>59</v>
       </c>
@@ -1248,8 +1392,11 @@
       <c r="G50" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D51" t="s">
         <v>18</v>
       </c>
@@ -1259,8 +1406,11 @@
       <c r="G51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H51" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>72</v>
       </c>
@@ -1271,7 +1421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D53" t="s">
         <v>23</v>
       </c>
@@ -1281,8 +1431,11 @@
       <c r="G53" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D54" t="s">
         <v>25</v>
       </c>
@@ -1292,8 +1445,11 @@
       <c r="G54" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H54" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D55" t="s">
         <v>59</v>
       </c>
@@ -1303,8 +1459,11 @@
       <c r="G55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H55" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D56" t="s">
         <v>18</v>
       </c>
@@ -1314,8 +1473,11 @@
       <c r="G56" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H56" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>73</v>
       </c>
@@ -1323,7 +1485,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>44</v>
       </c>
@@ -1333,8 +1495,11 @@
       <c r="G58" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D59" t="s">
         <v>45</v>
       </c>
@@ -1344,16 +1509,22 @@
       <c r="G59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D60" t="s">
         <v>59</v>
       </c>
       <c r="E60" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H60" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D61" t="s">
         <v>18</v>
       </c>
@@ -1363,8 +1534,11 @@
       <c r="G61" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H61" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -1372,7 +1546,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
         <v>68</v>
       </c>
@@ -1382,8 +1556,11 @@
       <c r="G63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H63" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="D64" t="s">
         <v>67</v>
       </c>
@@ -1393,24 +1570,36 @@
       <c r="G64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
         <v>59</v>
       </c>
       <c r="E65" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
         <v>18</v>
       </c>
       <c r="E66" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G66" t="s">
+        <v>117</v>
+      </c>
+      <c r="H66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -1418,26 +1607,32 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E68" t="s">
         <v>77</v>
       </c>
       <c r="G68" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="H68" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D69" t="s">
         <v>78</v>
       </c>
       <c r="E69" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D70" t="s">
         <v>18</v>
       </c>
@@ -1447,35 +1642,44 @@
       <c r="G70">
         <v>6</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B71" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D72" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D72" t="s">
-        <v>84</v>
       </c>
       <c r="E72" t="s">
         <v>77</v>
       </c>
       <c r="G72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+        <v>107</v>
+      </c>
+      <c r="H72" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D73" t="s">
         <v>78</v>
       </c>
       <c r="E73" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D74" t="s">
         <v>18</v>
       </c>
@@ -1483,37 +1687,46 @@
         <v>80</v>
       </c>
       <c r="G74" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H74" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D76" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>92</v>
-      </c>
-      <c r="B75" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D76" t="s">
-        <v>88</v>
       </c>
       <c r="E76" t="s">
         <v>77</v>
       </c>
       <c r="G76" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="H76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D77" t="s">
         <v>78</v>
       </c>
       <c r="E77" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D78" t="s">
         <v>18</v>
       </c>
@@ -1521,168 +1734,261 @@
         <v>80</v>
       </c>
       <c r="G78" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>93</v>
-      </c>
-      <c r="B79" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D80" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E80" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H80" t="s">
+        <v>116</v>
+      </c>
+      <c r="I80" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>78</v>
       </c>
       <c r="E81" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+      <c r="H81" t="s">
+        <v>116</v>
+      </c>
+      <c r="I81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>18</v>
       </c>
       <c r="E82" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" t="s">
+        <v>116</v>
+      </c>
+      <c r="I82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D84" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E84" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H84" t="s">
+        <v>116</v>
+      </c>
+      <c r="I84" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D85" t="s">
         <v>16</v>
       </c>
       <c r="E85" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="H85" t="s">
+        <v>116</v>
+      </c>
+      <c r="I85" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D86" t="s">
         <v>18</v>
       </c>
       <c r="E86" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="H86" t="s">
+        <v>116</v>
+      </c>
+      <c r="I86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B87" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D88" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E88" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H88" t="s">
+        <v>116</v>
+      </c>
+      <c r="I88" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D89" t="s">
         <v>29</v>
       </c>
       <c r="E89" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+      <c r="H89" t="s">
+        <v>116</v>
+      </c>
+      <c r="I89" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D90" t="s">
         <v>18</v>
       </c>
       <c r="E90" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="H90" t="s">
+        <v>116</v>
+      </c>
+      <c r="I90" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B91" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D92" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E92" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H92" t="s">
+        <v>116</v>
+      </c>
+      <c r="I92" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D93" t="s">
         <v>49</v>
       </c>
       <c r="E93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+      <c r="H93" t="s">
+        <v>116</v>
+      </c>
+      <c r="I93" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D94" t="s">
         <v>18</v>
       </c>
       <c r="E94" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+      <c r="H94" t="s">
+        <v>116</v>
+      </c>
+      <c r="I94" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="D96" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E96" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H96" t="s">
+        <v>116</v>
+      </c>
+      <c r="I96" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="97" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D97" t="s">
         <v>59</v>
       </c>
       <c r="E97" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+      <c r="H97" t="s">
+        <v>116</v>
+      </c>
+      <c r="I97" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="98" spans="4:9" x14ac:dyDescent="0.35">
       <c r="D98" t="s">
         <v>18</v>
       </c>
       <c r="E98" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="H98" t="s">
+        <v>116</v>
+      </c>
+      <c r="I98" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>